<commit_message>
add: add data expand result
</commit_message>
<xml_diff>
--- a/数据扩充/Atomic/Image.xlsx
+++ b/数据扩充/Atomic/Image.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyouyu/WorkSpace/Lab106/106Lab_Project/数据扩充/Atomic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF73EE47-FDFF-9141-B828-0EE8B018FAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D775BCA-79C8-244A-A81E-1AB448A3DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5000" windowWidth="51200" windowHeight="26760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>AN1</t>
   </si>
@@ -325,6 +325,10 @@
   </si>
   <si>
     <t>PHSS</t>
+  </si>
+  <si>
+    <t>zeros</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -669,7 +673,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -988,11 +992,11 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
+      <c r="G10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="I10" t="s">
         <v>80</v>
@@ -1020,17 +1024,17 @@
       <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
+      <c r="G11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>